<commit_message>
Added lat,long pairs for 4 institutions in Northern Ireland to excel spreadsheet and its csv counterpart. Removed misspelled csv file.
</commit_message>
<xml_diff>
--- a/lib/UK-academic-institutions-geodata.xlsx
+++ b/lib/UK-academic-institutions-geodata.xlsx
@@ -1,16 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="28028"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="20" windowWidth="22220" windowHeight="13880"/>
   </bookViews>
   <sheets>
     <sheet name="UK-academic-institutions" sheetId="1" r:id="rId1"/>
     <sheet name="ReadMe" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -4205,7 +4210,7 @@
     <t>It contains info on UK learning providers including information about the location of each institution.</t>
   </si>
   <si>
-    <t>Data in sheet 'UK-academic-institutons' was extracted on 2017-10-16 from http://learning-provider.data.ac.uk/.</t>
+    <t>Data in sheet 'UK-academic-institutons' was extracted on 2017-10-16 from http://learning-provider.data.ac.uk/ .</t>
   </si>
 </sst>
 </file>
@@ -4565,16 +4570,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T167"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="C100" workbookViewId="0">
+      <selection activeCell="Q133" sqref="Q133"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="40.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4636,7 +4641,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20">
       <c r="A2">
         <v>10008640</v>
       </c>
@@ -4686,7 +4691,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20">
       <c r="A3">
         <v>10007774</v>
       </c>
@@ -4739,7 +4744,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20">
       <c r="A4">
         <v>10007768</v>
       </c>
@@ -4792,7 +4797,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20">
       <c r="A5">
         <v>10000571</v>
       </c>
@@ -4845,7 +4850,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20">
       <c r="A6">
         <v>10007814</v>
       </c>
@@ -4895,7 +4900,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20">
       <c r="A7">
         <v>10007158</v>
       </c>
@@ -4945,7 +4950,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20">
       <c r="A8">
         <v>10007779</v>
       </c>
@@ -4992,7 +4997,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20">
       <c r="A9">
         <v>10007851</v>
       </c>
@@ -5042,7 +5047,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20">
       <c r="A10">
         <v>10000824</v>
       </c>
@@ -5098,7 +5103,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20">
       <c r="A11">
         <v>10007162</v>
       </c>
@@ -5148,7 +5153,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20">
       <c r="A12">
         <v>10007804</v>
       </c>
@@ -5192,7 +5197,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:20">
       <c r="A13">
         <v>10007823</v>
       </c>
@@ -5239,7 +5244,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:20">
       <c r="A14">
         <v>10007160</v>
       </c>
@@ -5283,7 +5288,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20">
       <c r="A15">
         <v>10007791</v>
       </c>
@@ -5333,7 +5338,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:20">
       <c r="A16">
         <v>10003945</v>
       </c>
@@ -5377,7 +5382,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20">
       <c r="A17">
         <v>10007802</v>
       </c>
@@ -5430,7 +5435,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:20">
       <c r="A18">
         <v>10007806</v>
       </c>
@@ -5486,7 +5491,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:20">
       <c r="A19">
         <v>10007152</v>
       </c>
@@ -5536,7 +5541,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:20">
       <c r="A20">
         <v>10007150</v>
       </c>
@@ -5586,7 +5591,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:20">
       <c r="A21">
         <v>10007832</v>
       </c>
@@ -5633,7 +5638,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:20">
       <c r="A22">
         <v>10007788</v>
       </c>
@@ -5686,7 +5691,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:20">
       <c r="A23">
         <v>10001883</v>
       </c>
@@ -5736,7 +5741,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:20">
       <c r="A24">
         <v>10007790</v>
       </c>
@@ -5789,7 +5794,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:20">
       <c r="A25">
         <v>10007795</v>
       </c>
@@ -5839,7 +5844,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:20">
       <c r="A26">
         <v>10008816</v>
       </c>
@@ -5884,7 +5889,7 @@
       </c>
       <c r="T26" s="2"/>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:20">
       <c r="A27">
         <v>10005343</v>
       </c>
@@ -5915,6 +5920,12 @@
       <c r="N27" t="s">
         <v>261</v>
       </c>
+      <c r="O27">
+        <v>-5.9348000000000001</v>
+      </c>
+      <c r="P27">
+        <v>54.5839</v>
+      </c>
       <c r="S27" t="s">
         <v>262</v>
       </c>
@@ -5922,7 +5933,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:20">
       <c r="A28">
         <v>10003861</v>
       </c>
@@ -5972,7 +5983,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:20">
       <c r="A29">
         <v>10007772</v>
       </c>
@@ -6025,7 +6036,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:20">
       <c r="A30">
         <v>10007854</v>
       </c>
@@ -6078,7 +6089,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:20">
       <c r="A31">
         <v>10007849</v>
       </c>
@@ -6131,7 +6142,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:20">
       <c r="A32">
         <v>10007164</v>
       </c>
@@ -6184,7 +6195,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:20">
       <c r="A33">
         <v>10007761</v>
       </c>
@@ -6234,7 +6245,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:20">
       <c r="A34">
         <v>10000961</v>
       </c>
@@ -6281,7 +6292,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:20">
       <c r="A35">
         <v>10007778</v>
       </c>
@@ -6328,7 +6339,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:20">
       <c r="A36">
         <v>10004180</v>
       </c>
@@ -6381,7 +6392,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:20">
       <c r="A37">
         <v>10007811</v>
       </c>
@@ -6431,7 +6442,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:20">
       <c r="A38">
         <v>10005389</v>
       </c>
@@ -6478,7 +6489,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:20">
       <c r="A39">
         <v>10003678</v>
       </c>
@@ -6531,7 +6542,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:20">
       <c r="A40">
         <v>10007166</v>
       </c>
@@ -6581,7 +6592,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:20">
       <c r="A41">
         <v>10001478</v>
       </c>
@@ -6628,7 +6639,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:20">
       <c r="A42">
         <v>10007781</v>
       </c>
@@ -6676,7 +6687,7 @@
       </c>
       <c r="T42" s="2"/>
     </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:20">
       <c r="A43">
         <v>10006427</v>
       </c>
@@ -6723,7 +6734,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:20">
       <c r="A44">
         <v>10008026</v>
       </c>
@@ -6754,6 +6765,12 @@
       <c r="M44" t="s">
         <v>401</v>
       </c>
+      <c r="O44">
+        <v>-5.9612999999999996</v>
+      </c>
+      <c r="P44">
+        <v>54.591999999999999</v>
+      </c>
       <c r="S44" t="s">
         <v>402</v>
       </c>
@@ -6761,7 +6778,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:20">
       <c r="A45">
         <v>10005500</v>
       </c>
@@ -6811,7 +6828,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:20">
       <c r="A46">
         <v>10008017</v>
       </c>
@@ -6861,7 +6878,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:20">
       <c r="A47">
         <v>10007114</v>
       </c>
@@ -6911,7 +6928,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:20">
       <c r="A48">
         <v>10007775</v>
       </c>
@@ -6964,7 +6981,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:20">
       <c r="A49">
         <v>10007144</v>
       </c>
@@ -7017,7 +7034,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:20">
       <c r="A50">
         <v>10002718</v>
       </c>
@@ -7070,7 +7087,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:20">
       <c r="A51">
         <v>10007797</v>
       </c>
@@ -7120,7 +7137,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:20">
       <c r="A52">
         <v>10007161</v>
       </c>
@@ -7170,7 +7187,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="53" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:20">
       <c r="A53">
         <v>10001282</v>
       </c>
@@ -7223,7 +7240,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:20">
       <c r="A54">
         <v>10006299</v>
       </c>
@@ -7273,7 +7290,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:20">
       <c r="A55">
         <v>10007145</v>
       </c>
@@ -7323,7 +7340,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:20">
       <c r="A56">
         <v>10007140</v>
       </c>
@@ -7376,7 +7393,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="57" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:20">
       <c r="A57">
         <v>10007816</v>
       </c>
@@ -7426,7 +7443,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="58" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:20">
       <c r="A58">
         <v>10007794</v>
       </c>
@@ -7476,7 +7493,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="59" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:20">
       <c r="A59">
         <v>10001726</v>
       </c>
@@ -7526,7 +7543,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="60" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:20">
       <c r="A60">
         <v>10007155</v>
       </c>
@@ -7579,7 +7596,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="61" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:20">
       <c r="A61">
         <v>10040812</v>
       </c>
@@ -7626,7 +7643,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="62" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:20">
       <c r="A62">
         <v>10034449</v>
       </c>
@@ -7671,7 +7688,7 @@
       </c>
       <c r="T62" s="2"/>
     </row>
-    <row r="63" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:20">
       <c r="A63">
         <v>10002681</v>
       </c>
@@ -7721,7 +7738,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="64" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:20">
       <c r="A64">
         <v>10007856</v>
       </c>
@@ -7771,7 +7788,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="65" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:20">
       <c r="A65">
         <v>10003614</v>
       </c>
@@ -7821,7 +7838,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="66" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:20">
       <c r="A66">
         <v>10007801</v>
       </c>
@@ -7871,7 +7888,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="67" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:20">
       <c r="A67">
         <v>10007789</v>
       </c>
@@ -7924,7 +7941,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="68" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:20">
       <c r="A68">
         <v>10007786</v>
       </c>
@@ -7977,7 +7994,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="69" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:20">
       <c r="A69">
         <v>10007803</v>
       </c>
@@ -8027,7 +8044,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="70" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:20">
       <c r="A70">
         <v>10006841</v>
       </c>
@@ -8077,7 +8094,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="71" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:20">
       <c r="A71">
         <v>10005337</v>
       </c>
@@ -8124,7 +8141,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="72" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:20">
       <c r="A72">
         <v>10007807</v>
       </c>
@@ -8155,6 +8172,12 @@
       <c r="N72" t="s">
         <v>198</v>
       </c>
+      <c r="O72">
+        <v>-6.6725000000000003</v>
+      </c>
+      <c r="P72">
+        <v>55.146799999999999</v>
+      </c>
       <c r="S72" t="s">
         <v>644</v>
       </c>
@@ -8162,7 +8185,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="73" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:20">
       <c r="A73">
         <v>10007163</v>
       </c>
@@ -8215,7 +8238,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="74" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:20">
       <c r="A74">
         <v>10007138</v>
       </c>
@@ -8262,7 +8285,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="75" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:20">
       <c r="A75">
         <v>10007796</v>
       </c>
@@ -8312,7 +8335,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="76" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:20">
       <c r="A76">
         <v>10000712</v>
       </c>
@@ -8356,7 +8379,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="77" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:20">
       <c r="A77">
         <v>10007762</v>
       </c>
@@ -8409,7 +8432,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="78" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:20">
       <c r="A78">
         <v>10007165</v>
       </c>
@@ -8459,7 +8482,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="79" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:20">
       <c r="A79">
         <v>10007148</v>
       </c>
@@ -8509,7 +8532,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="80" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:20">
       <c r="A80">
         <v>10005545</v>
       </c>
@@ -8553,7 +8576,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="81" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:20">
       <c r="A81">
         <v>10007765</v>
       </c>
@@ -8603,7 +8626,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="82" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:20">
       <c r="A82">
         <v>10007838</v>
       </c>
@@ -8645,7 +8668,7 @@
       </c>
       <c r="T82" s="2"/>
     </row>
-    <row r="83" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:20">
       <c r="A83">
         <v>10005523</v>
       </c>
@@ -8689,7 +8712,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="84" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:20">
       <c r="A84">
         <v>10007156</v>
       </c>
@@ -8742,7 +8765,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="85" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:20">
       <c r="A85">
         <v>10007657</v>
       </c>
@@ -8792,7 +8815,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="86" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:20">
       <c r="A86">
         <v>10004063</v>
       </c>
@@ -8842,7 +8865,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="87" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:20">
       <c r="A87">
         <v>10004351</v>
       </c>
@@ -8892,7 +8915,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="88" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:20">
       <c r="A88">
         <v>10007773</v>
       </c>
@@ -8942,7 +8965,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:20">
       <c r="A89">
         <v>10006022</v>
       </c>
@@ -8992,7 +9015,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="90" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:20">
       <c r="A90">
         <v>10000975</v>
       </c>
@@ -9042,7 +9065,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="91" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:20">
       <c r="A91">
         <v>10007167</v>
       </c>
@@ -9092,7 +9115,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="92" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:20">
       <c r="A92">
         <v>10007151</v>
       </c>
@@ -9142,7 +9165,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="93" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:20">
       <c r="A93">
         <v>10007784</v>
       </c>
@@ -9192,7 +9215,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="94" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:20">
       <c r="A94">
         <v>10000886</v>
       </c>
@@ -9242,7 +9265,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="95" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:20">
       <c r="A95">
         <v>10004113</v>
       </c>
@@ -9289,7 +9312,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="96" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:20">
       <c r="A96">
         <v>10007833</v>
       </c>
@@ -9339,7 +9362,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="97" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:20">
       <c r="A97">
         <v>10007771</v>
       </c>
@@ -9386,7 +9409,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="98" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:20">
       <c r="A98">
         <v>10003956</v>
       </c>
@@ -9439,7 +9462,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="99" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:20">
       <c r="A99">
         <v>10007147</v>
       </c>
@@ -9489,7 +9512,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="100" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:20">
       <c r="A100">
         <v>10007157</v>
       </c>
@@ -9539,7 +9562,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="101" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:20">
       <c r="A101">
         <v>10007143</v>
       </c>
@@ -9592,7 +9615,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="102" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:20">
       <c r="A102">
         <v>10004797</v>
       </c>
@@ -9642,7 +9665,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="103" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:20">
       <c r="A103">
         <v>10007805</v>
       </c>
@@ -9692,7 +9715,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="104" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:20">
       <c r="A104">
         <v>10007137</v>
       </c>
@@ -9745,7 +9768,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="105" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:20">
       <c r="A105">
         <v>10007764</v>
       </c>
@@ -9792,7 +9815,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="106" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:20">
       <c r="A106">
         <v>10007769</v>
       </c>
@@ -9839,7 +9862,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="107" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:20">
       <c r="A107">
         <v>10006840</v>
       </c>
@@ -9889,7 +9912,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="108" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:20">
       <c r="A108">
         <v>10007842</v>
       </c>
@@ -9939,7 +9962,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="109" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:20">
       <c r="A109">
         <v>10007792</v>
       </c>
@@ -9989,7 +10012,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="110" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:20">
       <c r="A110">
         <v>10005790</v>
       </c>
@@ -10042,7 +10065,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="111" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:20">
       <c r="A111">
         <v>10007852</v>
       </c>
@@ -10089,7 +10112,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="112" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:20">
       <c r="A112">
         <v>10005700</v>
       </c>
@@ -10136,7 +10159,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="113" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:20">
       <c r="A113">
         <v>10007776</v>
       </c>
@@ -10189,7 +10212,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="114" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:20">
       <c r="A114">
         <v>10007159</v>
       </c>
@@ -10239,7 +10262,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="115" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:20">
       <c r="A115">
         <v>10000291</v>
       </c>
@@ -10289,7 +10312,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="116" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:20">
       <c r="A116">
         <v>10007766</v>
       </c>
@@ -10342,7 +10365,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="117" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:20">
       <c r="A117">
         <v>10007855</v>
       </c>
@@ -10389,7 +10412,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="118" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:20">
       <c r="A118">
         <v>10005553</v>
       </c>
@@ -10439,7 +10462,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="119" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:20">
       <c r="A119">
         <v>10007777</v>
       </c>
@@ -10486,7 +10509,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="120" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:20">
       <c r="A120">
         <v>10007822</v>
       </c>
@@ -10536,7 +10559,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="121" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:20">
       <c r="A121">
         <v>10007767</v>
       </c>
@@ -10583,7 +10606,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="122" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:20">
       <c r="A122">
         <v>10003863</v>
       </c>
@@ -10633,7 +10656,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="123" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:20">
       <c r="A123">
         <v>10003645</v>
       </c>
@@ -10683,7 +10706,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="124" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:20">
       <c r="A124">
         <v>10007782</v>
       </c>
@@ -10730,7 +10753,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="125" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:20">
       <c r="A125">
         <v>10004775</v>
       </c>
@@ -10780,7 +10803,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="126" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:20">
       <c r="A126">
         <v>10003854</v>
       </c>
@@ -10824,7 +10847,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="127" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:20">
       <c r="A127">
         <v>10007759</v>
       </c>
@@ -10874,7 +10897,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="128" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:20">
       <c r="A128">
         <v>10007848</v>
       </c>
@@ -10924,7 +10947,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="129" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:20">
       <c r="A129">
         <v>10007783</v>
       </c>
@@ -10971,7 +10994,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="130" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:20">
       <c r="A130">
         <v>10007798</v>
       </c>
@@ -11021,7 +11044,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="131" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:20">
       <c r="A131">
         <v>10005561</v>
       </c>
@@ -11068,7 +11091,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="132" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:20">
       <c r="A132">
         <v>10007154</v>
       </c>
@@ -11118,7 +11141,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="133" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:20">
       <c r="A133">
         <v>10008010</v>
       </c>
@@ -11146,11 +11169,17 @@
       <c r="M133" t="s">
         <v>1128</v>
       </c>
+      <c r="O133">
+        <v>-5.9352</v>
+      </c>
+      <c r="P133">
+        <v>54.573300000000003</v>
+      </c>
       <c r="T133" s="2">
         <v>193</v>
       </c>
     </row>
-    <row r="134" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:20">
       <c r="A134">
         <v>10007799</v>
       </c>
@@ -11200,7 +11229,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="135" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:20">
       <c r="A135">
         <v>10007857</v>
       </c>
@@ -11250,7 +11279,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="136" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:20">
       <c r="A136">
         <v>10037449</v>
       </c>
@@ -11300,7 +11329,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="137" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:20">
       <c r="A137">
         <v>10007787</v>
       </c>
@@ -11350,7 +11379,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="138" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:20">
       <c r="A138">
         <v>10007149</v>
       </c>
@@ -11397,7 +11426,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="139" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:20">
       <c r="A139">
         <v>10007793</v>
       </c>
@@ -11447,7 +11476,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="140" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:20">
       <c r="A140">
         <v>10007835</v>
       </c>
@@ -11494,7 +11523,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="141" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:20">
       <c r="A141">
         <v>10004048</v>
       </c>
@@ -11547,7 +11576,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="142" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:20">
       <c r="A142">
         <v>10007843</v>
       </c>
@@ -11597,7 +11626,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="143" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:20">
       <c r="A143">
         <v>10001143</v>
       </c>
@@ -11647,7 +11676,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="144" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:20">
       <c r="A144">
         <v>10001653</v>
       </c>
@@ -11694,7 +11723,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="145" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:20">
       <c r="A145">
         <v>10007760</v>
       </c>
@@ -11747,7 +11776,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="146" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:20">
       <c r="A146">
         <v>10006842</v>
       </c>
@@ -11797,7 +11826,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="147" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:20">
       <c r="A147">
         <v>10003324</v>
       </c>
@@ -11847,7 +11876,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="148" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:20">
       <c r="A148">
         <v>10007146</v>
       </c>
@@ -11900,7 +11929,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="149" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:20">
       <c r="A149">
         <v>10007713</v>
       </c>
@@ -11950,7 +11979,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="150" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:20">
       <c r="A150">
         <v>10007858</v>
       </c>
@@ -11997,7 +12026,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="151" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:20">
       <c r="A151">
         <v>10007846</v>
       </c>
@@ -12045,7 +12074,7 @@
       </c>
       <c r="T151" s="2"/>
     </row>
-    <row r="152" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:20">
       <c r="A152">
         <v>10007825</v>
       </c>
@@ -12092,7 +12121,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="153" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:20">
       <c r="A153">
         <v>10007785</v>
       </c>
@@ -12142,7 +12171,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="154" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:20">
       <c r="A154">
         <v>10004078</v>
       </c>
@@ -12192,7 +12221,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="155" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:20">
       <c r="A155">
         <v>10014001</v>
       </c>
@@ -12239,7 +12268,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="156" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:20">
       <c r="A156">
         <v>10007800</v>
       </c>
@@ -12289,7 +12318,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="157" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:20">
       <c r="A157">
         <v>10003957</v>
       </c>
@@ -12342,7 +12371,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="158" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:20">
       <c r="A158">
         <v>10007850</v>
       </c>
@@ -12392,7 +12421,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="159" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:20">
       <c r="A159">
         <v>10000385</v>
       </c>
@@ -12442,7 +12471,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="160" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:20">
       <c r="A160">
         <v>10006566</v>
       </c>
@@ -12492,7 +12521,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="161" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:20">
       <c r="A161">
         <v>10004930</v>
       </c>
@@ -12545,7 +12574,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="162" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:20">
       <c r="A162">
         <v>10007780</v>
       </c>
@@ -12598,7 +12627,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="163" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:20">
       <c r="A163">
         <v>10007837</v>
       </c>
@@ -12648,7 +12677,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="164" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:20">
       <c r="A164">
         <v>10007141</v>
       </c>
@@ -12695,7 +12724,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="165" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:20">
       <c r="A165">
         <v>10003270</v>
       </c>
@@ -12748,7 +12777,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="166" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:20">
       <c r="A166">
         <v>10008574</v>
       </c>
@@ -12795,7 +12824,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="167" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:20">
       <c r="A167">
         <v>10007139</v>
       </c>
@@ -13112,72 +13141,76 @@
     <hyperlink ref="M134" r:id="rId266"/>
     <hyperlink ref="L135" r:id="rId267"/>
     <hyperlink ref="M135" r:id="rId268"/>
-    <hyperlink ref="L136" r:id="rId269"/>
-    <hyperlink ref="M136" r:id="rId270"/>
-    <hyperlink ref="L137" r:id="rId271"/>
-    <hyperlink ref="M137" r:id="rId272"/>
-    <hyperlink ref="L138" r:id="rId273"/>
-    <hyperlink ref="M138" r:id="rId274"/>
-    <hyperlink ref="L139" r:id="rId275"/>
-    <hyperlink ref="M139" r:id="rId276"/>
-    <hyperlink ref="L140" r:id="rId277"/>
-    <hyperlink ref="M140" r:id="rId278"/>
-    <hyperlink ref="L141" r:id="rId279"/>
-    <hyperlink ref="M141" r:id="rId280"/>
-    <hyperlink ref="L142" r:id="rId281"/>
-    <hyperlink ref="M142" r:id="rId282"/>
-    <hyperlink ref="L143" r:id="rId283"/>
-    <hyperlink ref="M143" r:id="rId284"/>
-    <hyperlink ref="L144" r:id="rId285"/>
-    <hyperlink ref="M144" r:id="rId286"/>
-    <hyperlink ref="L145" r:id="rId287"/>
-    <hyperlink ref="M145" r:id="rId288"/>
-    <hyperlink ref="L146" r:id="rId289"/>
-    <hyperlink ref="M146" r:id="rId290"/>
-    <hyperlink ref="L147" r:id="rId291"/>
-    <hyperlink ref="M147" r:id="rId292"/>
-    <hyperlink ref="L148" r:id="rId293"/>
-    <hyperlink ref="M148" r:id="rId294"/>
-    <hyperlink ref="L149" r:id="rId295"/>
-    <hyperlink ref="M149" r:id="rId296"/>
-    <hyperlink ref="L150" r:id="rId297"/>
-    <hyperlink ref="M150" r:id="rId298"/>
-    <hyperlink ref="L151" r:id="rId299"/>
-    <hyperlink ref="M151" r:id="rId300"/>
-    <hyperlink ref="L152" r:id="rId301"/>
-    <hyperlink ref="M152" r:id="rId302"/>
-    <hyperlink ref="L153" r:id="rId303"/>
-    <hyperlink ref="M153" r:id="rId304"/>
-    <hyperlink ref="L154" r:id="rId305"/>
-    <hyperlink ref="M154" r:id="rId306"/>
-    <hyperlink ref="L155" r:id="rId307"/>
-    <hyperlink ref="M155" r:id="rId308"/>
-    <hyperlink ref="L156" r:id="rId309"/>
-    <hyperlink ref="M156" r:id="rId310"/>
-    <hyperlink ref="L157" r:id="rId311"/>
-    <hyperlink ref="M157" r:id="rId312"/>
-    <hyperlink ref="L158" r:id="rId313"/>
-    <hyperlink ref="M158" r:id="rId314"/>
-    <hyperlink ref="L159" r:id="rId315"/>
-    <hyperlink ref="M159" r:id="rId316"/>
-    <hyperlink ref="L160" r:id="rId317"/>
-    <hyperlink ref="M160" r:id="rId318"/>
-    <hyperlink ref="L161" r:id="rId319"/>
-    <hyperlink ref="M161" r:id="rId320"/>
-    <hyperlink ref="L162" r:id="rId321"/>
-    <hyperlink ref="M162" r:id="rId322"/>
-    <hyperlink ref="L163" r:id="rId323"/>
-    <hyperlink ref="M163" r:id="rId324"/>
-    <hyperlink ref="L164" r:id="rId325"/>
-    <hyperlink ref="M164" r:id="rId326"/>
-    <hyperlink ref="L165" r:id="rId327"/>
-    <hyperlink ref="M165" r:id="rId328"/>
-    <hyperlink ref="L166" r:id="rId329"/>
-    <hyperlink ref="M166" r:id="rId330"/>
-    <hyperlink ref="L167" r:id="rId331"/>
-    <hyperlink ref="M167" r:id="rId332"/>
+    <hyperlink ref="M136" r:id="rId269"/>
+    <hyperlink ref="L137" r:id="rId270"/>
+    <hyperlink ref="M137" r:id="rId271"/>
+    <hyperlink ref="L138" r:id="rId272"/>
+    <hyperlink ref="M138" r:id="rId273"/>
+    <hyperlink ref="L139" r:id="rId274"/>
+    <hyperlink ref="M139" r:id="rId275"/>
+    <hyperlink ref="L140" r:id="rId276"/>
+    <hyperlink ref="M140" r:id="rId277"/>
+    <hyperlink ref="L141" r:id="rId278"/>
+    <hyperlink ref="M141" r:id="rId279"/>
+    <hyperlink ref="L142" r:id="rId280"/>
+    <hyperlink ref="M142" r:id="rId281"/>
+    <hyperlink ref="L143" r:id="rId282"/>
+    <hyperlink ref="M143" r:id="rId283"/>
+    <hyperlink ref="L144" r:id="rId284"/>
+    <hyperlink ref="M144" r:id="rId285"/>
+    <hyperlink ref="L145" r:id="rId286"/>
+    <hyperlink ref="M145" r:id="rId287"/>
+    <hyperlink ref="L146" r:id="rId288"/>
+    <hyperlink ref="M146" r:id="rId289"/>
+    <hyperlink ref="L147" r:id="rId290"/>
+    <hyperlink ref="M147" r:id="rId291"/>
+    <hyperlink ref="L148" r:id="rId292"/>
+    <hyperlink ref="M148" r:id="rId293"/>
+    <hyperlink ref="L149" r:id="rId294"/>
+    <hyperlink ref="M149" r:id="rId295"/>
+    <hyperlink ref="L150" r:id="rId296"/>
+    <hyperlink ref="M150" r:id="rId297"/>
+    <hyperlink ref="L151" r:id="rId298"/>
+    <hyperlink ref="M151" r:id="rId299"/>
+    <hyperlink ref="L152" r:id="rId300"/>
+    <hyperlink ref="M152" r:id="rId301"/>
+    <hyperlink ref="L153" r:id="rId302"/>
+    <hyperlink ref="M153" r:id="rId303"/>
+    <hyperlink ref="L154" r:id="rId304"/>
+    <hyperlink ref="M154" r:id="rId305"/>
+    <hyperlink ref="L155" r:id="rId306"/>
+    <hyperlink ref="M155" r:id="rId307"/>
+    <hyperlink ref="L156" r:id="rId308"/>
+    <hyperlink ref="M156" r:id="rId309"/>
+    <hyperlink ref="L157" r:id="rId310"/>
+    <hyperlink ref="M157" r:id="rId311"/>
+    <hyperlink ref="L158" r:id="rId312"/>
+    <hyperlink ref="M158" r:id="rId313"/>
+    <hyperlink ref="L159" r:id="rId314"/>
+    <hyperlink ref="M159" r:id="rId315"/>
+    <hyperlink ref="L160" r:id="rId316"/>
+    <hyperlink ref="M160" r:id="rId317"/>
+    <hyperlink ref="L161" r:id="rId318"/>
+    <hyperlink ref="M161" r:id="rId319"/>
+    <hyperlink ref="L162" r:id="rId320"/>
+    <hyperlink ref="M162" r:id="rId321"/>
+    <hyperlink ref="L163" r:id="rId322"/>
+    <hyperlink ref="M163" r:id="rId323"/>
+    <hyperlink ref="L164" r:id="rId324"/>
+    <hyperlink ref="M164" r:id="rId325"/>
+    <hyperlink ref="L165" r:id="rId326"/>
+    <hyperlink ref="M165" r:id="rId327"/>
+    <hyperlink ref="L166" r:id="rId328"/>
+    <hyperlink ref="M166" r:id="rId329"/>
+    <hyperlink ref="L167" r:id="rId330"/>
+    <hyperlink ref="M167" r:id="rId331"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -13185,23 +13218,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
         <v>1396</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1">
       <c r="A3" t="s">
         <v>1395</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Check Missing coordinates and add readme note
</commit_message>
<xml_diff>
--- a/lib/UK-academic-institutions-geodata.xlsx
+++ b/lib/UK-academic-institutions-geodata.xlsx
@@ -2,20 +2,25 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="24" windowWidth="22224" windowHeight="13176" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="UK-academic-institutions" sheetId="1" r:id="rId1"/>
     <sheet name="ReadMe" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1652" uniqueCount="1397">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1653" uniqueCount="1398">
   <si>
     <t>UKPRN</t>
   </si>
@@ -4205,7 +4210,10 @@
     <t>It contains info on UK learning providers including information about the location of each institution.</t>
   </si>
   <si>
-    <t>Data in sheet 'UK-academic-institutons' was extracted on 2017-10-16 from http://learning-provider.data.ac.uk/.</t>
+    <t>Data in sheet 'UK-academic-institutons' was extracted on 2017-10-16 from http://learning-provider.data.ac.uk/ .</t>
+  </si>
+  <si>
+    <t>The coordinates for The Queen's University of Belfast, St Mary's University College, University of Ulster and Stranmillis University College were added manually to this file.</t>
   </si>
 </sst>
 </file>
@@ -4565,11 +4573,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T167"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView topLeftCell="C100" workbookViewId="0">
+      <selection activeCell="Q133" sqref="Q133"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="40.6640625" customWidth="1"/>
   </cols>
@@ -5915,6 +5923,12 @@
       <c r="N27" t="s">
         <v>261</v>
       </c>
+      <c r="O27">
+        <v>-5.9348000000000001</v>
+      </c>
+      <c r="P27">
+        <v>54.5839</v>
+      </c>
       <c r="S27" t="s">
         <v>262</v>
       </c>
@@ -6754,6 +6768,12 @@
       <c r="M44" t="s">
         <v>401</v>
       </c>
+      <c r="O44">
+        <v>-5.9612999999999996</v>
+      </c>
+      <c r="P44">
+        <v>54.591999999999999</v>
+      </c>
       <c r="S44" t="s">
         <v>402</v>
       </c>
@@ -8155,6 +8175,12 @@
       <c r="N72" t="s">
         <v>198</v>
       </c>
+      <c r="O72">
+        <v>-6.6725000000000003</v>
+      </c>
+      <c r="P72">
+        <v>55.146799999999999</v>
+      </c>
       <c r="S72" t="s">
         <v>644</v>
       </c>
@@ -11145,6 +11171,12 @@
       </c>
       <c r="M133" t="s">
         <v>1128</v>
+      </c>
+      <c r="O133">
+        <v>-5.9352</v>
+      </c>
+      <c r="P133">
+        <v>54.573300000000003</v>
       </c>
       <c r="T133" s="2">
         <v>193</v>
@@ -13112,84 +13144,88 @@
     <hyperlink ref="M134" r:id="rId266"/>
     <hyperlink ref="L135" r:id="rId267"/>
     <hyperlink ref="M135" r:id="rId268"/>
-    <hyperlink ref="L136" r:id="rId269"/>
-    <hyperlink ref="M136" r:id="rId270"/>
-    <hyperlink ref="L137" r:id="rId271"/>
-    <hyperlink ref="M137" r:id="rId272"/>
-    <hyperlink ref="L138" r:id="rId273"/>
-    <hyperlink ref="M138" r:id="rId274"/>
-    <hyperlink ref="L139" r:id="rId275"/>
-    <hyperlink ref="M139" r:id="rId276"/>
-    <hyperlink ref="L140" r:id="rId277"/>
-    <hyperlink ref="M140" r:id="rId278"/>
-    <hyperlink ref="L141" r:id="rId279"/>
-    <hyperlink ref="M141" r:id="rId280"/>
-    <hyperlink ref="L142" r:id="rId281"/>
-    <hyperlink ref="M142" r:id="rId282"/>
-    <hyperlink ref="L143" r:id="rId283"/>
-    <hyperlink ref="M143" r:id="rId284"/>
-    <hyperlink ref="L144" r:id="rId285"/>
-    <hyperlink ref="M144" r:id="rId286"/>
-    <hyperlink ref="L145" r:id="rId287"/>
-    <hyperlink ref="M145" r:id="rId288"/>
-    <hyperlink ref="L146" r:id="rId289"/>
-    <hyperlink ref="M146" r:id="rId290"/>
-    <hyperlink ref="L147" r:id="rId291"/>
-    <hyperlink ref="M147" r:id="rId292"/>
-    <hyperlink ref="L148" r:id="rId293"/>
-    <hyperlink ref="M148" r:id="rId294"/>
-    <hyperlink ref="L149" r:id="rId295"/>
-    <hyperlink ref="M149" r:id="rId296"/>
-    <hyperlink ref="L150" r:id="rId297"/>
-    <hyperlink ref="M150" r:id="rId298"/>
-    <hyperlink ref="L151" r:id="rId299"/>
-    <hyperlink ref="M151" r:id="rId300"/>
-    <hyperlink ref="L152" r:id="rId301"/>
-    <hyperlink ref="M152" r:id="rId302"/>
-    <hyperlink ref="L153" r:id="rId303"/>
-    <hyperlink ref="M153" r:id="rId304"/>
-    <hyperlink ref="L154" r:id="rId305"/>
-    <hyperlink ref="M154" r:id="rId306"/>
-    <hyperlink ref="L155" r:id="rId307"/>
-    <hyperlink ref="M155" r:id="rId308"/>
-    <hyperlink ref="L156" r:id="rId309"/>
-    <hyperlink ref="M156" r:id="rId310"/>
-    <hyperlink ref="L157" r:id="rId311"/>
-    <hyperlink ref="M157" r:id="rId312"/>
-    <hyperlink ref="L158" r:id="rId313"/>
-    <hyperlink ref="M158" r:id="rId314"/>
-    <hyperlink ref="L159" r:id="rId315"/>
-    <hyperlink ref="M159" r:id="rId316"/>
-    <hyperlink ref="L160" r:id="rId317"/>
-    <hyperlink ref="M160" r:id="rId318"/>
-    <hyperlink ref="L161" r:id="rId319"/>
-    <hyperlink ref="M161" r:id="rId320"/>
-    <hyperlink ref="L162" r:id="rId321"/>
-    <hyperlink ref="M162" r:id="rId322"/>
-    <hyperlink ref="L163" r:id="rId323"/>
-    <hyperlink ref="M163" r:id="rId324"/>
-    <hyperlink ref="L164" r:id="rId325"/>
-    <hyperlink ref="M164" r:id="rId326"/>
-    <hyperlink ref="L165" r:id="rId327"/>
-    <hyperlink ref="M165" r:id="rId328"/>
-    <hyperlink ref="L166" r:id="rId329"/>
-    <hyperlink ref="M166" r:id="rId330"/>
-    <hyperlink ref="L167" r:id="rId331"/>
-    <hyperlink ref="M167" r:id="rId332"/>
+    <hyperlink ref="M136" r:id="rId269"/>
+    <hyperlink ref="L137" r:id="rId270"/>
+    <hyperlink ref="M137" r:id="rId271"/>
+    <hyperlink ref="L138" r:id="rId272"/>
+    <hyperlink ref="M138" r:id="rId273"/>
+    <hyperlink ref="L139" r:id="rId274"/>
+    <hyperlink ref="M139" r:id="rId275"/>
+    <hyperlink ref="L140" r:id="rId276"/>
+    <hyperlink ref="M140" r:id="rId277"/>
+    <hyperlink ref="L141" r:id="rId278"/>
+    <hyperlink ref="M141" r:id="rId279"/>
+    <hyperlink ref="L142" r:id="rId280"/>
+    <hyperlink ref="M142" r:id="rId281"/>
+    <hyperlink ref="L143" r:id="rId282"/>
+    <hyperlink ref="M143" r:id="rId283"/>
+    <hyperlink ref="L144" r:id="rId284"/>
+    <hyperlink ref="M144" r:id="rId285"/>
+    <hyperlink ref="L145" r:id="rId286"/>
+    <hyperlink ref="M145" r:id="rId287"/>
+    <hyperlink ref="L146" r:id="rId288"/>
+    <hyperlink ref="M146" r:id="rId289"/>
+    <hyperlink ref="L147" r:id="rId290"/>
+    <hyperlink ref="M147" r:id="rId291"/>
+    <hyperlink ref="L148" r:id="rId292"/>
+    <hyperlink ref="M148" r:id="rId293"/>
+    <hyperlink ref="L149" r:id="rId294"/>
+    <hyperlink ref="M149" r:id="rId295"/>
+    <hyperlink ref="L150" r:id="rId296"/>
+    <hyperlink ref="M150" r:id="rId297"/>
+    <hyperlink ref="L151" r:id="rId298"/>
+    <hyperlink ref="M151" r:id="rId299"/>
+    <hyperlink ref="L152" r:id="rId300"/>
+    <hyperlink ref="M152" r:id="rId301"/>
+    <hyperlink ref="L153" r:id="rId302"/>
+    <hyperlink ref="M153" r:id="rId303"/>
+    <hyperlink ref="L154" r:id="rId304"/>
+    <hyperlink ref="M154" r:id="rId305"/>
+    <hyperlink ref="L155" r:id="rId306"/>
+    <hyperlink ref="M155" r:id="rId307"/>
+    <hyperlink ref="L156" r:id="rId308"/>
+    <hyperlink ref="M156" r:id="rId309"/>
+    <hyperlink ref="L157" r:id="rId310"/>
+    <hyperlink ref="M157" r:id="rId311"/>
+    <hyperlink ref="L158" r:id="rId312"/>
+    <hyperlink ref="M158" r:id="rId313"/>
+    <hyperlink ref="L159" r:id="rId314"/>
+    <hyperlink ref="M159" r:id="rId315"/>
+    <hyperlink ref="L160" r:id="rId316"/>
+    <hyperlink ref="M160" r:id="rId317"/>
+    <hyperlink ref="L161" r:id="rId318"/>
+    <hyperlink ref="M161" r:id="rId319"/>
+    <hyperlink ref="L162" r:id="rId320"/>
+    <hyperlink ref="M162" r:id="rId321"/>
+    <hyperlink ref="L163" r:id="rId322"/>
+    <hyperlink ref="M163" r:id="rId323"/>
+    <hyperlink ref="L164" r:id="rId324"/>
+    <hyperlink ref="M164" r:id="rId325"/>
+    <hyperlink ref="L165" r:id="rId326"/>
+    <hyperlink ref="M165" r:id="rId327"/>
+    <hyperlink ref="L166" r:id="rId328"/>
+    <hyperlink ref="M166" r:id="rId329"/>
+    <hyperlink ref="L167" r:id="rId330"/>
+    <hyperlink ref="M167" r:id="rId331"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -13201,7 +13237,17 @@
         <v>1395</v>
       </c>
     </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>1397</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated UK academic institutions file
</commit_message>
<xml_diff>
--- a/lib/UK-academic-institutions-geodata.xlsx
+++ b/lib/UK-academic-institutions-geodata.xlsx
@@ -2,25 +2,20 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="24" windowWidth="22224" windowHeight="13176" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="UK-academic-institutions" sheetId="1" r:id="rId1"/>
     <sheet name="ReadMe" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1653" uniqueCount="1398">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1652" uniqueCount="1397">
   <si>
     <t>UKPRN</t>
   </si>
@@ -1105,7 +1100,7 @@
     <t>http://en.wikipedia.org/wiki/Kingston_University</t>
   </si>
   <si>
-    <t>NCUK, University_Alliance</t>
+    <t>University_Alliance, NCUK</t>
   </si>
   <si>
     <t>6E750E7A-C076-435E-8AB0-484F65D6C7AD</t>
@@ -1843,7 +1838,7 @@
     <t>http://en.wikipedia.org/wiki/University_of_Bristol</t>
   </si>
   <si>
-    <t>NCUK, GW4, Russell_Group</t>
+    <t>GW4, NCUK, Russell_Group</t>
   </si>
   <si>
     <t>FD94FDDE-5BBC-4E12-911F-0B70DBCFA743</t>
@@ -4210,10 +4205,7 @@
     <t>It contains info on UK learning providers including information about the location of each institution.</t>
   </si>
   <si>
-    <t>Data in sheet 'UK-academic-institutons' was extracted on 2017-10-16 from http://learning-provider.data.ac.uk/ .</t>
-  </si>
-  <si>
-    <t>The coordinates for The Queen's University of Belfast, St Mary's University College, University of Ulster and Stranmillis University College were added manually to this file.</t>
+    <t>Data in sheet 'UK-academic-institutons' was extracted on 2017-10-27 from http://learning-provider.data.ac.uk/</t>
   </si>
 </sst>
 </file>
@@ -4573,11 +4565,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T167"/>
   <sheetViews>
-    <sheetView topLeftCell="C100" workbookViewId="0">
-      <selection activeCell="Q133" sqref="Q133"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="40.6640625" customWidth="1"/>
   </cols>
@@ -13144,88 +13134,84 @@
     <hyperlink ref="M134" r:id="rId266"/>
     <hyperlink ref="L135" r:id="rId267"/>
     <hyperlink ref="M135" r:id="rId268"/>
-    <hyperlink ref="M136" r:id="rId269"/>
-    <hyperlink ref="L137" r:id="rId270"/>
-    <hyperlink ref="M137" r:id="rId271"/>
-    <hyperlink ref="L138" r:id="rId272"/>
-    <hyperlink ref="M138" r:id="rId273"/>
-    <hyperlink ref="L139" r:id="rId274"/>
-    <hyperlink ref="M139" r:id="rId275"/>
-    <hyperlink ref="L140" r:id="rId276"/>
-    <hyperlink ref="M140" r:id="rId277"/>
-    <hyperlink ref="L141" r:id="rId278"/>
-    <hyperlink ref="M141" r:id="rId279"/>
-    <hyperlink ref="L142" r:id="rId280"/>
-    <hyperlink ref="M142" r:id="rId281"/>
-    <hyperlink ref="L143" r:id="rId282"/>
-    <hyperlink ref="M143" r:id="rId283"/>
-    <hyperlink ref="L144" r:id="rId284"/>
-    <hyperlink ref="M144" r:id="rId285"/>
-    <hyperlink ref="L145" r:id="rId286"/>
-    <hyperlink ref="M145" r:id="rId287"/>
-    <hyperlink ref="L146" r:id="rId288"/>
-    <hyperlink ref="M146" r:id="rId289"/>
-    <hyperlink ref="L147" r:id="rId290"/>
-    <hyperlink ref="M147" r:id="rId291"/>
-    <hyperlink ref="L148" r:id="rId292"/>
-    <hyperlink ref="M148" r:id="rId293"/>
-    <hyperlink ref="L149" r:id="rId294"/>
-    <hyperlink ref="M149" r:id="rId295"/>
-    <hyperlink ref="L150" r:id="rId296"/>
-    <hyperlink ref="M150" r:id="rId297"/>
-    <hyperlink ref="L151" r:id="rId298"/>
-    <hyperlink ref="M151" r:id="rId299"/>
-    <hyperlink ref="L152" r:id="rId300"/>
-    <hyperlink ref="M152" r:id="rId301"/>
-    <hyperlink ref="L153" r:id="rId302"/>
-    <hyperlink ref="M153" r:id="rId303"/>
-    <hyperlink ref="L154" r:id="rId304"/>
-    <hyperlink ref="M154" r:id="rId305"/>
-    <hyperlink ref="L155" r:id="rId306"/>
-    <hyperlink ref="M155" r:id="rId307"/>
-    <hyperlink ref="L156" r:id="rId308"/>
-    <hyperlink ref="M156" r:id="rId309"/>
-    <hyperlink ref="L157" r:id="rId310"/>
-    <hyperlink ref="M157" r:id="rId311"/>
-    <hyperlink ref="L158" r:id="rId312"/>
-    <hyperlink ref="M158" r:id="rId313"/>
-    <hyperlink ref="L159" r:id="rId314"/>
-    <hyperlink ref="M159" r:id="rId315"/>
-    <hyperlink ref="L160" r:id="rId316"/>
-    <hyperlink ref="M160" r:id="rId317"/>
-    <hyperlink ref="L161" r:id="rId318"/>
-    <hyperlink ref="M161" r:id="rId319"/>
-    <hyperlink ref="L162" r:id="rId320"/>
-    <hyperlink ref="M162" r:id="rId321"/>
-    <hyperlink ref="L163" r:id="rId322"/>
-    <hyperlink ref="M163" r:id="rId323"/>
-    <hyperlink ref="L164" r:id="rId324"/>
-    <hyperlink ref="M164" r:id="rId325"/>
-    <hyperlink ref="L165" r:id="rId326"/>
-    <hyperlink ref="M165" r:id="rId327"/>
-    <hyperlink ref="L166" r:id="rId328"/>
-    <hyperlink ref="M166" r:id="rId329"/>
-    <hyperlink ref="L167" r:id="rId330"/>
-    <hyperlink ref="M167" r:id="rId331"/>
+    <hyperlink ref="L136" r:id="rId269"/>
+    <hyperlink ref="M136" r:id="rId270"/>
+    <hyperlink ref="L137" r:id="rId271"/>
+    <hyperlink ref="M137" r:id="rId272"/>
+    <hyperlink ref="L138" r:id="rId273"/>
+    <hyperlink ref="M138" r:id="rId274"/>
+    <hyperlink ref="L139" r:id="rId275"/>
+    <hyperlink ref="M139" r:id="rId276"/>
+    <hyperlink ref="L140" r:id="rId277"/>
+    <hyperlink ref="M140" r:id="rId278"/>
+    <hyperlink ref="L141" r:id="rId279"/>
+    <hyperlink ref="M141" r:id="rId280"/>
+    <hyperlink ref="L142" r:id="rId281"/>
+    <hyperlink ref="M142" r:id="rId282"/>
+    <hyperlink ref="L143" r:id="rId283"/>
+    <hyperlink ref="M143" r:id="rId284"/>
+    <hyperlink ref="L144" r:id="rId285"/>
+    <hyperlink ref="M144" r:id="rId286"/>
+    <hyperlink ref="L145" r:id="rId287"/>
+    <hyperlink ref="M145" r:id="rId288"/>
+    <hyperlink ref="L146" r:id="rId289"/>
+    <hyperlink ref="M146" r:id="rId290"/>
+    <hyperlink ref="L147" r:id="rId291"/>
+    <hyperlink ref="M147" r:id="rId292"/>
+    <hyperlink ref="L148" r:id="rId293"/>
+    <hyperlink ref="M148" r:id="rId294"/>
+    <hyperlink ref="L149" r:id="rId295"/>
+    <hyperlink ref="M149" r:id="rId296"/>
+    <hyperlink ref="L150" r:id="rId297"/>
+    <hyperlink ref="M150" r:id="rId298"/>
+    <hyperlink ref="L151" r:id="rId299"/>
+    <hyperlink ref="M151" r:id="rId300"/>
+    <hyperlink ref="L152" r:id="rId301"/>
+    <hyperlink ref="M152" r:id="rId302"/>
+    <hyperlink ref="L153" r:id="rId303"/>
+    <hyperlink ref="M153" r:id="rId304"/>
+    <hyperlink ref="L154" r:id="rId305"/>
+    <hyperlink ref="M154" r:id="rId306"/>
+    <hyperlink ref="L155" r:id="rId307"/>
+    <hyperlink ref="M155" r:id="rId308"/>
+    <hyperlink ref="L156" r:id="rId309"/>
+    <hyperlink ref="M156" r:id="rId310"/>
+    <hyperlink ref="L157" r:id="rId311"/>
+    <hyperlink ref="M157" r:id="rId312"/>
+    <hyperlink ref="L158" r:id="rId313"/>
+    <hyperlink ref="M158" r:id="rId314"/>
+    <hyperlink ref="L159" r:id="rId315"/>
+    <hyperlink ref="M159" r:id="rId316"/>
+    <hyperlink ref="L160" r:id="rId317"/>
+    <hyperlink ref="M160" r:id="rId318"/>
+    <hyperlink ref="L161" r:id="rId319"/>
+    <hyperlink ref="M161" r:id="rId320"/>
+    <hyperlink ref="L162" r:id="rId321"/>
+    <hyperlink ref="M162" r:id="rId322"/>
+    <hyperlink ref="L163" r:id="rId323"/>
+    <hyperlink ref="M163" r:id="rId324"/>
+    <hyperlink ref="L164" r:id="rId325"/>
+    <hyperlink ref="M164" r:id="rId326"/>
+    <hyperlink ref="L165" r:id="rId327"/>
+    <hyperlink ref="M165" r:id="rId328"/>
+    <hyperlink ref="L166" r:id="rId329"/>
+    <hyperlink ref="M166" r:id="rId330"/>
+    <hyperlink ref="L167" r:id="rId331"/>
+    <hyperlink ref="M167" r:id="rId332"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -13237,17 +13223,7 @@
         <v>1395</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>1397</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
renamed ReadMe -> README in geocodes sheet.
</commit_message>
<xml_diff>
--- a/lib/UK-academic-institutions-geodata.xlsx
+++ b/lib/UK-academic-institutions-geodata.xlsx
@@ -1,16 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="28028"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="20" windowWidth="28820" windowHeight="18740"/>
   </bookViews>
   <sheets>
     <sheet name="UK-academic-institutions" sheetId="1" r:id="rId1"/>
-    <sheet name="ReadMe" sheetId="2" r:id="rId2"/>
+    <sheet name="README" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -4567,12 +4572,12 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="40.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4634,7 +4639,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20">
       <c r="A2">
         <v>10008640</v>
       </c>
@@ -4684,7 +4689,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20">
       <c r="A3">
         <v>10007774</v>
       </c>
@@ -4737,7 +4742,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20">
       <c r="A4">
         <v>10007768</v>
       </c>
@@ -4790,7 +4795,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20">
       <c r="A5">
         <v>10000571</v>
       </c>
@@ -4843,7 +4848,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20">
       <c r="A6">
         <v>10007814</v>
       </c>
@@ -4893,7 +4898,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20">
       <c r="A7">
         <v>10007158</v>
       </c>
@@ -4943,7 +4948,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20">
       <c r="A8">
         <v>10007779</v>
       </c>
@@ -4990,7 +4995,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20">
       <c r="A9">
         <v>10007851</v>
       </c>
@@ -5040,7 +5045,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20">
       <c r="A10">
         <v>10000824</v>
       </c>
@@ -5096,7 +5101,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20">
       <c r="A11">
         <v>10007162</v>
       </c>
@@ -5146,7 +5151,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20">
       <c r="A12">
         <v>10007804</v>
       </c>
@@ -5190,7 +5195,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:20">
       <c r="A13">
         <v>10007823</v>
       </c>
@@ -5237,7 +5242,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:20">
       <c r="A14">
         <v>10007160</v>
       </c>
@@ -5281,7 +5286,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20">
       <c r="A15">
         <v>10007791</v>
       </c>
@@ -5331,7 +5336,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:20">
       <c r="A16">
         <v>10003945</v>
       </c>
@@ -5375,7 +5380,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20">
       <c r="A17">
         <v>10007802</v>
       </c>
@@ -5428,7 +5433,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:20">
       <c r="A18">
         <v>10007806</v>
       </c>
@@ -5484,7 +5489,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:20">
       <c r="A19">
         <v>10007152</v>
       </c>
@@ -5534,7 +5539,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:20">
       <c r="A20">
         <v>10007150</v>
       </c>
@@ -5584,7 +5589,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:20">
       <c r="A21">
         <v>10007832</v>
       </c>
@@ -5631,7 +5636,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:20">
       <c r="A22">
         <v>10007788</v>
       </c>
@@ -5684,7 +5689,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:20">
       <c r="A23">
         <v>10001883</v>
       </c>
@@ -5734,7 +5739,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:20">
       <c r="A24">
         <v>10007790</v>
       </c>
@@ -5787,7 +5792,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:20">
       <c r="A25">
         <v>10007795</v>
       </c>
@@ -5837,7 +5842,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:20">
       <c r="A26">
         <v>10008816</v>
       </c>
@@ -5882,7 +5887,7 @@
       </c>
       <c r="T26" s="2"/>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:20">
       <c r="A27">
         <v>10005343</v>
       </c>
@@ -5926,7 +5931,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:20">
       <c r="A28">
         <v>10003861</v>
       </c>
@@ -5976,7 +5981,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:20">
       <c r="A29">
         <v>10007772</v>
       </c>
@@ -6029,7 +6034,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:20">
       <c r="A30">
         <v>10007854</v>
       </c>
@@ -6082,7 +6087,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:20">
       <c r="A31">
         <v>10007849</v>
       </c>
@@ -6135,7 +6140,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:20">
       <c r="A32">
         <v>10007164</v>
       </c>
@@ -6188,7 +6193,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:20">
       <c r="A33">
         <v>10007761</v>
       </c>
@@ -6238,7 +6243,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:20">
       <c r="A34">
         <v>10000961</v>
       </c>
@@ -6285,7 +6290,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:20">
       <c r="A35">
         <v>10007778</v>
       </c>
@@ -6332,7 +6337,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:20">
       <c r="A36">
         <v>10004180</v>
       </c>
@@ -6385,7 +6390,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:20">
       <c r="A37">
         <v>10007811</v>
       </c>
@@ -6435,7 +6440,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:20">
       <c r="A38">
         <v>10005389</v>
       </c>
@@ -6482,7 +6487,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:20">
       <c r="A39">
         <v>10003678</v>
       </c>
@@ -6535,7 +6540,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:20">
       <c r="A40">
         <v>10007166</v>
       </c>
@@ -6585,7 +6590,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:20">
       <c r="A41">
         <v>10001478</v>
       </c>
@@ -6632,7 +6637,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:20">
       <c r="A42">
         <v>10007781</v>
       </c>
@@ -6680,7 +6685,7 @@
       </c>
       <c r="T42" s="2"/>
     </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:20">
       <c r="A43">
         <v>10006427</v>
       </c>
@@ -6727,7 +6732,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:20">
       <c r="A44">
         <v>10008026</v>
       </c>
@@ -6771,7 +6776,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:20">
       <c r="A45">
         <v>10005500</v>
       </c>
@@ -6821,7 +6826,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:20">
       <c r="A46">
         <v>10008017</v>
       </c>
@@ -6871,7 +6876,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:20">
       <c r="A47">
         <v>10007114</v>
       </c>
@@ -6921,7 +6926,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:20">
       <c r="A48">
         <v>10007775</v>
       </c>
@@ -6974,7 +6979,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:20">
       <c r="A49">
         <v>10007144</v>
       </c>
@@ -7027,7 +7032,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:20">
       <c r="A50">
         <v>10002718</v>
       </c>
@@ -7080,7 +7085,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:20">
       <c r="A51">
         <v>10007797</v>
       </c>
@@ -7130,7 +7135,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:20">
       <c r="A52">
         <v>10007161</v>
       </c>
@@ -7180,7 +7185,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="53" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:20">
       <c r="A53">
         <v>10001282</v>
       </c>
@@ -7233,7 +7238,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:20">
       <c r="A54">
         <v>10006299</v>
       </c>
@@ -7283,7 +7288,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:20">
       <c r="A55">
         <v>10007145</v>
       </c>
@@ -7333,7 +7338,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:20">
       <c r="A56">
         <v>10007140</v>
       </c>
@@ -7386,7 +7391,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="57" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:20">
       <c r="A57">
         <v>10007816</v>
       </c>
@@ -7436,7 +7441,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="58" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:20">
       <c r="A58">
         <v>10007794</v>
       </c>
@@ -7486,7 +7491,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="59" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:20">
       <c r="A59">
         <v>10001726</v>
       </c>
@@ -7536,7 +7541,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="60" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:20">
       <c r="A60">
         <v>10007155</v>
       </c>
@@ -7589,7 +7594,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="61" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:20">
       <c r="A61">
         <v>10040812</v>
       </c>
@@ -7636,7 +7641,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="62" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:20">
       <c r="A62">
         <v>10034449</v>
       </c>
@@ -7681,7 +7686,7 @@
       </c>
       <c r="T62" s="2"/>
     </row>
-    <row r="63" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:20">
       <c r="A63">
         <v>10002681</v>
       </c>
@@ -7731,7 +7736,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="64" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:20">
       <c r="A64">
         <v>10007856</v>
       </c>
@@ -7781,7 +7786,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="65" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:20">
       <c r="A65">
         <v>10003614</v>
       </c>
@@ -7831,7 +7836,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="66" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:20">
       <c r="A66">
         <v>10007801</v>
       </c>
@@ -7881,7 +7886,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="67" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:20">
       <c r="A67">
         <v>10007789</v>
       </c>
@@ -7934,7 +7939,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="68" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:20">
       <c r="A68">
         <v>10007786</v>
       </c>
@@ -7987,7 +7992,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="69" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:20">
       <c r="A69">
         <v>10007803</v>
       </c>
@@ -8037,7 +8042,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="70" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:20">
       <c r="A70">
         <v>10006841</v>
       </c>
@@ -8087,7 +8092,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="71" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:20">
       <c r="A71">
         <v>10005337</v>
       </c>
@@ -8134,7 +8139,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="72" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:20">
       <c r="A72">
         <v>10007807</v>
       </c>
@@ -8178,7 +8183,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="73" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:20">
       <c r="A73">
         <v>10007163</v>
       </c>
@@ -8231,7 +8236,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="74" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:20">
       <c r="A74">
         <v>10007138</v>
       </c>
@@ -8278,7 +8283,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="75" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:20">
       <c r="A75">
         <v>10007796</v>
       </c>
@@ -8328,7 +8333,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="76" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:20">
       <c r="A76">
         <v>10000712</v>
       </c>
@@ -8372,7 +8377,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="77" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:20">
       <c r="A77">
         <v>10007762</v>
       </c>
@@ -8425,7 +8430,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="78" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:20">
       <c r="A78">
         <v>10007165</v>
       </c>
@@ -8475,7 +8480,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="79" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:20">
       <c r="A79">
         <v>10007148</v>
       </c>
@@ -8525,7 +8530,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="80" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:20">
       <c r="A80">
         <v>10005545</v>
       </c>
@@ -8569,7 +8574,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="81" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:20">
       <c r="A81">
         <v>10007765</v>
       </c>
@@ -8619,7 +8624,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="82" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:20">
       <c r="A82">
         <v>10007838</v>
       </c>
@@ -8661,7 +8666,7 @@
       </c>
       <c r="T82" s="2"/>
     </row>
-    <row r="83" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:20">
       <c r="A83">
         <v>10005523</v>
       </c>
@@ -8705,7 +8710,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="84" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:20">
       <c r="A84">
         <v>10007156</v>
       </c>
@@ -8758,7 +8763,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="85" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:20">
       <c r="A85">
         <v>10007657</v>
       </c>
@@ -8808,7 +8813,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="86" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:20">
       <c r="A86">
         <v>10004063</v>
       </c>
@@ -8858,7 +8863,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="87" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:20">
       <c r="A87">
         <v>10004351</v>
       </c>
@@ -8908,7 +8913,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="88" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:20">
       <c r="A88">
         <v>10007773</v>
       </c>
@@ -8958,7 +8963,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:20">
       <c r="A89">
         <v>10006022</v>
       </c>
@@ -9008,7 +9013,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="90" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:20">
       <c r="A90">
         <v>10000975</v>
       </c>
@@ -9058,7 +9063,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="91" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:20">
       <c r="A91">
         <v>10007167</v>
       </c>
@@ -9108,7 +9113,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="92" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:20">
       <c r="A92">
         <v>10007151</v>
       </c>
@@ -9158,7 +9163,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="93" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:20">
       <c r="A93">
         <v>10007784</v>
       </c>
@@ -9208,7 +9213,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="94" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:20">
       <c r="A94">
         <v>10000886</v>
       </c>
@@ -9258,7 +9263,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="95" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:20">
       <c r="A95">
         <v>10004113</v>
       </c>
@@ -9305,7 +9310,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="96" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:20">
       <c r="A96">
         <v>10007833</v>
       </c>
@@ -9355,7 +9360,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="97" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:20">
       <c r="A97">
         <v>10007771</v>
       </c>
@@ -9402,7 +9407,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="98" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:20">
       <c r="A98">
         <v>10003956</v>
       </c>
@@ -9455,7 +9460,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="99" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:20">
       <c r="A99">
         <v>10007147</v>
       </c>
@@ -9505,7 +9510,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="100" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:20">
       <c r="A100">
         <v>10007157</v>
       </c>
@@ -9555,7 +9560,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="101" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:20">
       <c r="A101">
         <v>10007143</v>
       </c>
@@ -9608,7 +9613,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="102" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:20">
       <c r="A102">
         <v>10004797</v>
       </c>
@@ -9658,7 +9663,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="103" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:20">
       <c r="A103">
         <v>10007805</v>
       </c>
@@ -9708,7 +9713,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="104" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:20">
       <c r="A104">
         <v>10007137</v>
       </c>
@@ -9761,7 +9766,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="105" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:20">
       <c r="A105">
         <v>10007764</v>
       </c>
@@ -9808,7 +9813,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="106" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:20">
       <c r="A106">
         <v>10007769</v>
       </c>
@@ -9855,7 +9860,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="107" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:20">
       <c r="A107">
         <v>10006840</v>
       </c>
@@ -9905,7 +9910,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="108" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:20">
       <c r="A108">
         <v>10007842</v>
       </c>
@@ -9955,7 +9960,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="109" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:20">
       <c r="A109">
         <v>10007792</v>
       </c>
@@ -10005,7 +10010,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="110" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:20">
       <c r="A110">
         <v>10005790</v>
       </c>
@@ -10058,7 +10063,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="111" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:20">
       <c r="A111">
         <v>10007852</v>
       </c>
@@ -10105,7 +10110,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="112" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:20">
       <c r="A112">
         <v>10005700</v>
       </c>
@@ -10152,7 +10157,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="113" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:20">
       <c r="A113">
         <v>10007776</v>
       </c>
@@ -10205,7 +10210,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="114" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:20">
       <c r="A114">
         <v>10007159</v>
       </c>
@@ -10255,7 +10260,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="115" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:20">
       <c r="A115">
         <v>10000291</v>
       </c>
@@ -10305,7 +10310,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="116" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:20">
       <c r="A116">
         <v>10007766</v>
       </c>
@@ -10358,7 +10363,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="117" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:20">
       <c r="A117">
         <v>10007855</v>
       </c>
@@ -10405,7 +10410,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="118" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:20">
       <c r="A118">
         <v>10005553</v>
       </c>
@@ -10455,7 +10460,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="119" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:20">
       <c r="A119">
         <v>10007777</v>
       </c>
@@ -10502,7 +10507,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="120" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:20">
       <c r="A120">
         <v>10007822</v>
       </c>
@@ -10552,7 +10557,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="121" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:20">
       <c r="A121">
         <v>10007767</v>
       </c>
@@ -10599,7 +10604,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="122" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:20">
       <c r="A122">
         <v>10003863</v>
       </c>
@@ -10649,7 +10654,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="123" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:20">
       <c r="A123">
         <v>10003645</v>
       </c>
@@ -10699,7 +10704,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="124" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:20">
       <c r="A124">
         <v>10007782</v>
       </c>
@@ -10746,7 +10751,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="125" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:20">
       <c r="A125">
         <v>10004775</v>
       </c>
@@ -10796,7 +10801,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="126" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:20">
       <c r="A126">
         <v>10003854</v>
       </c>
@@ -10840,7 +10845,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="127" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:20">
       <c r="A127">
         <v>10007759</v>
       </c>
@@ -10890,7 +10895,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="128" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:20">
       <c r="A128">
         <v>10007848</v>
       </c>
@@ -10940,7 +10945,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="129" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:20">
       <c r="A129">
         <v>10007783</v>
       </c>
@@ -10987,7 +10992,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="130" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:20">
       <c r="A130">
         <v>10007798</v>
       </c>
@@ -11037,7 +11042,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="131" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:20">
       <c r="A131">
         <v>10005561</v>
       </c>
@@ -11084,7 +11089,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="132" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:20">
       <c r="A132">
         <v>10007154</v>
       </c>
@@ -11134,7 +11139,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="133" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:20">
       <c r="A133">
         <v>10008010</v>
       </c>
@@ -11172,7 +11177,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="134" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:20">
       <c r="A134">
         <v>10007799</v>
       </c>
@@ -11222,7 +11227,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="135" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:20">
       <c r="A135">
         <v>10007857</v>
       </c>
@@ -11272,7 +11277,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="136" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:20">
       <c r="A136">
         <v>10037449</v>
       </c>
@@ -11322,7 +11327,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="137" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:20">
       <c r="A137">
         <v>10007787</v>
       </c>
@@ -11372,7 +11377,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="138" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:20">
       <c r="A138">
         <v>10007149</v>
       </c>
@@ -11419,7 +11424,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="139" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:20">
       <c r="A139">
         <v>10007793</v>
       </c>
@@ -11469,7 +11474,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="140" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:20">
       <c r="A140">
         <v>10007835</v>
       </c>
@@ -11516,7 +11521,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="141" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:20">
       <c r="A141">
         <v>10004048</v>
       </c>
@@ -11569,7 +11574,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="142" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:20">
       <c r="A142">
         <v>10007843</v>
       </c>
@@ -11619,7 +11624,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="143" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:20">
       <c r="A143">
         <v>10001143</v>
       </c>
@@ -11669,7 +11674,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="144" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:20">
       <c r="A144">
         <v>10001653</v>
       </c>
@@ -11716,7 +11721,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="145" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:20">
       <c r="A145">
         <v>10007760</v>
       </c>
@@ -11769,7 +11774,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="146" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:20">
       <c r="A146">
         <v>10006842</v>
       </c>
@@ -11819,7 +11824,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="147" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:20">
       <c r="A147">
         <v>10003324</v>
       </c>
@@ -11869,7 +11874,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="148" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:20">
       <c r="A148">
         <v>10007146</v>
       </c>
@@ -11922,7 +11927,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="149" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:20">
       <c r="A149">
         <v>10007713</v>
       </c>
@@ -11972,7 +11977,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="150" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:20">
       <c r="A150">
         <v>10007858</v>
       </c>
@@ -12019,7 +12024,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="151" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:20">
       <c r="A151">
         <v>10007846</v>
       </c>
@@ -12067,7 +12072,7 @@
       </c>
       <c r="T151" s="2"/>
     </row>
-    <row r="152" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:20">
       <c r="A152">
         <v>10007825</v>
       </c>
@@ -12114,7 +12119,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="153" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:20">
       <c r="A153">
         <v>10007785</v>
       </c>
@@ -12164,7 +12169,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="154" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:20">
       <c r="A154">
         <v>10004078</v>
       </c>
@@ -12214,7 +12219,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="155" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:20">
       <c r="A155">
         <v>10014001</v>
       </c>
@@ -12261,7 +12266,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="156" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:20">
       <c r="A156">
         <v>10007800</v>
       </c>
@@ -12311,7 +12316,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="157" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:20">
       <c r="A157">
         <v>10003957</v>
       </c>
@@ -12364,7 +12369,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="158" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:20">
       <c r="A158">
         <v>10007850</v>
       </c>
@@ -12414,7 +12419,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="159" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:20">
       <c r="A159">
         <v>10000385</v>
       </c>
@@ -12464,7 +12469,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="160" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:20">
       <c r="A160">
         <v>10006566</v>
       </c>
@@ -12514,7 +12519,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="161" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:20">
       <c r="A161">
         <v>10004930</v>
       </c>
@@ -12567,7 +12572,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="162" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:20">
       <c r="A162">
         <v>10007780</v>
       </c>
@@ -12620,7 +12625,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="163" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:20">
       <c r="A163">
         <v>10007837</v>
       </c>
@@ -12670,7 +12675,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="164" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:20">
       <c r="A164">
         <v>10007141</v>
       </c>
@@ -12717,7 +12722,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="165" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:20">
       <c r="A165">
         <v>10003270</v>
       </c>
@@ -12770,7 +12775,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="166" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:20">
       <c r="A166">
         <v>10008574</v>
       </c>
@@ -12817,7 +12822,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="167" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:20">
       <c r="A167">
         <v>10007139</v>
       </c>
@@ -13134,72 +13139,76 @@
     <hyperlink ref="M134" r:id="rId266"/>
     <hyperlink ref="L135" r:id="rId267"/>
     <hyperlink ref="M135" r:id="rId268"/>
-    <hyperlink ref="L136" r:id="rId269"/>
-    <hyperlink ref="M136" r:id="rId270"/>
-    <hyperlink ref="L137" r:id="rId271"/>
-    <hyperlink ref="M137" r:id="rId272"/>
-    <hyperlink ref="L138" r:id="rId273"/>
-    <hyperlink ref="M138" r:id="rId274"/>
-    <hyperlink ref="L139" r:id="rId275"/>
-    <hyperlink ref="M139" r:id="rId276"/>
-    <hyperlink ref="L140" r:id="rId277"/>
-    <hyperlink ref="M140" r:id="rId278"/>
-    <hyperlink ref="L141" r:id="rId279"/>
-    <hyperlink ref="M141" r:id="rId280"/>
-    <hyperlink ref="L142" r:id="rId281"/>
-    <hyperlink ref="M142" r:id="rId282"/>
-    <hyperlink ref="L143" r:id="rId283"/>
-    <hyperlink ref="M143" r:id="rId284"/>
-    <hyperlink ref="L144" r:id="rId285"/>
-    <hyperlink ref="M144" r:id="rId286"/>
-    <hyperlink ref="L145" r:id="rId287"/>
-    <hyperlink ref="M145" r:id="rId288"/>
-    <hyperlink ref="L146" r:id="rId289"/>
-    <hyperlink ref="M146" r:id="rId290"/>
-    <hyperlink ref="L147" r:id="rId291"/>
-    <hyperlink ref="M147" r:id="rId292"/>
-    <hyperlink ref="L148" r:id="rId293"/>
-    <hyperlink ref="M148" r:id="rId294"/>
-    <hyperlink ref="L149" r:id="rId295"/>
-    <hyperlink ref="M149" r:id="rId296"/>
-    <hyperlink ref="L150" r:id="rId297"/>
-    <hyperlink ref="M150" r:id="rId298"/>
-    <hyperlink ref="L151" r:id="rId299"/>
-    <hyperlink ref="M151" r:id="rId300"/>
-    <hyperlink ref="L152" r:id="rId301"/>
-    <hyperlink ref="M152" r:id="rId302"/>
-    <hyperlink ref="L153" r:id="rId303"/>
-    <hyperlink ref="M153" r:id="rId304"/>
-    <hyperlink ref="L154" r:id="rId305"/>
-    <hyperlink ref="M154" r:id="rId306"/>
-    <hyperlink ref="L155" r:id="rId307"/>
-    <hyperlink ref="M155" r:id="rId308"/>
-    <hyperlink ref="L156" r:id="rId309"/>
-    <hyperlink ref="M156" r:id="rId310"/>
-    <hyperlink ref="L157" r:id="rId311"/>
-    <hyperlink ref="M157" r:id="rId312"/>
-    <hyperlink ref="L158" r:id="rId313"/>
-    <hyperlink ref="M158" r:id="rId314"/>
-    <hyperlink ref="L159" r:id="rId315"/>
-    <hyperlink ref="M159" r:id="rId316"/>
-    <hyperlink ref="L160" r:id="rId317"/>
-    <hyperlink ref="M160" r:id="rId318"/>
-    <hyperlink ref="L161" r:id="rId319"/>
-    <hyperlink ref="M161" r:id="rId320"/>
-    <hyperlink ref="L162" r:id="rId321"/>
-    <hyperlink ref="M162" r:id="rId322"/>
-    <hyperlink ref="L163" r:id="rId323"/>
-    <hyperlink ref="M163" r:id="rId324"/>
-    <hyperlink ref="L164" r:id="rId325"/>
-    <hyperlink ref="M164" r:id="rId326"/>
-    <hyperlink ref="L165" r:id="rId327"/>
-    <hyperlink ref="M165" r:id="rId328"/>
-    <hyperlink ref="L166" r:id="rId329"/>
-    <hyperlink ref="M166" r:id="rId330"/>
-    <hyperlink ref="L167" r:id="rId331"/>
-    <hyperlink ref="M167" r:id="rId332"/>
+    <hyperlink ref="M136" r:id="rId269"/>
+    <hyperlink ref="L137" r:id="rId270"/>
+    <hyperlink ref="M137" r:id="rId271"/>
+    <hyperlink ref="L138" r:id="rId272"/>
+    <hyperlink ref="M138" r:id="rId273"/>
+    <hyperlink ref="L139" r:id="rId274"/>
+    <hyperlink ref="M139" r:id="rId275"/>
+    <hyperlink ref="L140" r:id="rId276"/>
+    <hyperlink ref="M140" r:id="rId277"/>
+    <hyperlink ref="L141" r:id="rId278"/>
+    <hyperlink ref="M141" r:id="rId279"/>
+    <hyperlink ref="L142" r:id="rId280"/>
+    <hyperlink ref="M142" r:id="rId281"/>
+    <hyperlink ref="L143" r:id="rId282"/>
+    <hyperlink ref="M143" r:id="rId283"/>
+    <hyperlink ref="L144" r:id="rId284"/>
+    <hyperlink ref="M144" r:id="rId285"/>
+    <hyperlink ref="L145" r:id="rId286"/>
+    <hyperlink ref="M145" r:id="rId287"/>
+    <hyperlink ref="L146" r:id="rId288"/>
+    <hyperlink ref="M146" r:id="rId289"/>
+    <hyperlink ref="L147" r:id="rId290"/>
+    <hyperlink ref="M147" r:id="rId291"/>
+    <hyperlink ref="L148" r:id="rId292"/>
+    <hyperlink ref="M148" r:id="rId293"/>
+    <hyperlink ref="L149" r:id="rId294"/>
+    <hyperlink ref="M149" r:id="rId295"/>
+    <hyperlink ref="L150" r:id="rId296"/>
+    <hyperlink ref="M150" r:id="rId297"/>
+    <hyperlink ref="L151" r:id="rId298"/>
+    <hyperlink ref="M151" r:id="rId299"/>
+    <hyperlink ref="L152" r:id="rId300"/>
+    <hyperlink ref="M152" r:id="rId301"/>
+    <hyperlink ref="L153" r:id="rId302"/>
+    <hyperlink ref="M153" r:id="rId303"/>
+    <hyperlink ref="L154" r:id="rId304"/>
+    <hyperlink ref="M154" r:id="rId305"/>
+    <hyperlink ref="L155" r:id="rId306"/>
+    <hyperlink ref="M155" r:id="rId307"/>
+    <hyperlink ref="L156" r:id="rId308"/>
+    <hyperlink ref="M156" r:id="rId309"/>
+    <hyperlink ref="L157" r:id="rId310"/>
+    <hyperlink ref="M157" r:id="rId311"/>
+    <hyperlink ref="L158" r:id="rId312"/>
+    <hyperlink ref="M158" r:id="rId313"/>
+    <hyperlink ref="L159" r:id="rId314"/>
+    <hyperlink ref="M159" r:id="rId315"/>
+    <hyperlink ref="L160" r:id="rId316"/>
+    <hyperlink ref="M160" r:id="rId317"/>
+    <hyperlink ref="L161" r:id="rId318"/>
+    <hyperlink ref="M161" r:id="rId319"/>
+    <hyperlink ref="L162" r:id="rId320"/>
+    <hyperlink ref="M162" r:id="rId321"/>
+    <hyperlink ref="L163" r:id="rId322"/>
+    <hyperlink ref="M163" r:id="rId323"/>
+    <hyperlink ref="L164" r:id="rId324"/>
+    <hyperlink ref="M164" r:id="rId325"/>
+    <hyperlink ref="L165" r:id="rId326"/>
+    <hyperlink ref="M165" r:id="rId327"/>
+    <hyperlink ref="L166" r:id="rId328"/>
+    <hyperlink ref="M166" r:id="rId329"/>
+    <hyperlink ref="L167" r:id="rId330"/>
+    <hyperlink ref="M167" r:id="rId331"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -13211,19 +13220,24 @@
       <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
         <v>1396</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1">
       <c r="A3" t="s">
         <v>1395</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>